<commit_message>
cierre 24 FEB 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/ENTRADAS OBRADOR FEBRERO  2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/ENTRADAS OBRADOR FEBRERO  2022.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="131">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -410,6 +410,15 @@
   </si>
   <si>
     <t>Transferencia  B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGROPECUARIA EL TOPETE   </t>
+  </si>
+  <si>
+    <t>CANALES 249</t>
+  </si>
+  <si>
+    <t>AGROPECUARIA EL TAPETE  250</t>
   </si>
 </sst>
 </file>
@@ -2809,111 +2818,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="32" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2925,30 +2832,6 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2971,6 +2854,132 @@
     </xf>
     <xf numFmtId="1" fontId="22" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3299,18 +3308,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="420" t="s">
+      <c r="A1" s="455" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="420"/>
-      <c r="C1" s="420"/>
-      <c r="D1" s="420"/>
-      <c r="E1" s="420"/>
-      <c r="F1" s="420"/>
-      <c r="G1" s="420"/>
-      <c r="H1" s="420"/>
-      <c r="I1" s="420"/>
-      <c r="J1" s="420"/>
+      <c r="B1" s="455"/>
+      <c r="C1" s="455"/>
+      <c r="D1" s="455"/>
+      <c r="E1" s="455"/>
+      <c r="F1" s="455"/>
+      <c r="G1" s="455"/>
+      <c r="H1" s="455"/>
+      <c r="I1" s="455"/>
+      <c r="J1" s="455"/>
       <c r="K1" s="377"/>
       <c r="L1" s="377"/>
       <c r="M1" s="377"/>
@@ -3324,22 +3333,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="421" t="s">
+      <c r="W1" s="456" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="422"/>
+      <c r="X1" s="457"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="420"/>
-      <c r="B2" s="420"/>
-      <c r="C2" s="420"/>
-      <c r="D2" s="420"/>
-      <c r="E2" s="420"/>
-      <c r="F2" s="420"/>
-      <c r="G2" s="420"/>
-      <c r="H2" s="420"/>
-      <c r="I2" s="420"/>
-      <c r="J2" s="420"/>
+      <c r="A2" s="455"/>
+      <c r="B2" s="455"/>
+      <c r="C2" s="455"/>
+      <c r="D2" s="455"/>
+      <c r="E2" s="455"/>
+      <c r="F2" s="455"/>
+      <c r="G2" s="455"/>
+      <c r="H2" s="455"/>
+      <c r="I2" s="455"/>
+      <c r="J2" s="455"/>
       <c r="K2" s="379"/>
       <c r="L2" s="379"/>
       <c r="M2" s="379"/>
@@ -3393,10 +3402,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="423" t="s">
+      <c r="O3" s="458" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="424"/>
+      <c r="P3" s="459"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -3908,7 +3917,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="435" t="s">
+      <c r="C12" s="460" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="402"/>
@@ -3968,7 +3977,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="436"/>
+      <c r="C13" s="461"/>
       <c r="D13" s="402"/>
       <c r="E13" s="403"/>
       <c r="F13" s="404">
@@ -4356,10 +4365,10 @@
         <f t="shared" si="1"/>
         <v>790920</v>
       </c>
-      <c r="O19" s="469" t="s">
+      <c r="O19" s="427" t="s">
         <v>61</v>
       </c>
-      <c r="P19" s="471">
+      <c r="P19" s="429">
         <v>44595</v>
       </c>
       <c r="Q19" s="79">
@@ -4416,10 +4425,10 @@
         <f t="shared" si="1"/>
         <v>206820</v>
       </c>
-      <c r="O20" s="469" t="s">
+      <c r="O20" s="427" t="s">
         <v>61</v>
       </c>
-      <c r="P20" s="471">
+      <c r="P20" s="429">
         <v>44595</v>
       </c>
       <c r="Q20" s="79">
@@ -4476,10 +4485,10 @@
         <f t="shared" si="1"/>
         <v>804600</v>
       </c>
-      <c r="O21" s="470" t="s">
+      <c r="O21" s="428" t="s">
         <v>61</v>
       </c>
-      <c r="P21" s="471">
+      <c r="P21" s="429">
         <v>44596</v>
       </c>
       <c r="Q21" s="79">
@@ -4536,10 +4545,10 @@
         <f t="shared" si="1"/>
         <v>195120</v>
       </c>
-      <c r="O22" s="470" t="s">
+      <c r="O22" s="428" t="s">
         <v>61</v>
       </c>
-      <c r="P22" s="471">
+      <c r="P22" s="429">
         <v>44596</v>
       </c>
       <c r="Q22" s="79">
@@ -4596,10 +4605,10 @@
         <f t="shared" si="1"/>
         <v>822240</v>
       </c>
-      <c r="O23" s="470" t="s">
+      <c r="O23" s="428" t="s">
         <v>61</v>
       </c>
-      <c r="P23" s="471">
+      <c r="P23" s="429">
         <v>44600</v>
       </c>
       <c r="Q23" s="79">
@@ -4656,10 +4665,10 @@
         <f t="shared" si="1"/>
         <v>195480</v>
       </c>
-      <c r="O24" s="469" t="s">
+      <c r="O24" s="427" t="s">
         <v>61</v>
       </c>
-      <c r="P24" s="471">
+      <c r="P24" s="429">
         <v>44600</v>
       </c>
       <c r="Q24" s="79">
@@ -4717,10 +4726,10 @@
         <f t="shared" si="1"/>
         <v>781711.55999999994</v>
       </c>
-      <c r="O25" s="470" t="s">
+      <c r="O25" s="428" t="s">
         <v>61</v>
       </c>
-      <c r="P25" s="471">
+      <c r="P25" s="429">
         <v>44600</v>
       </c>
       <c r="Q25" s="79">
@@ -4777,10 +4786,10 @@
         <f t="shared" si="1"/>
         <v>806382.5</v>
       </c>
-      <c r="O26" s="470" t="s">
+      <c r="O26" s="428" t="s">
         <v>61</v>
       </c>
-      <c r="P26" s="471">
+      <c r="P26" s="429">
         <v>44602</v>
       </c>
       <c r="Q26" s="79">
@@ -4837,10 +4846,10 @@
         <f t="shared" si="1"/>
         <v>813400</v>
       </c>
-      <c r="O27" s="470" t="s">
+      <c r="O27" s="428" t="s">
         <v>127</v>
       </c>
-      <c r="P27" s="471">
+      <c r="P27" s="429">
         <v>44603</v>
       </c>
       <c r="Q27" s="79">
@@ -4897,10 +4906,10 @@
         <f t="shared" si="1"/>
         <v>194425</v>
       </c>
-      <c r="O28" s="470" t="s">
+      <c r="O28" s="428" t="s">
         <v>61</v>
       </c>
-      <c r="P28" s="471">
+      <c r="P28" s="429">
         <v>44603</v>
       </c>
       <c r="Q28" s="66">
@@ -4938,7 +4947,7 @@
       <c r="G29" s="62">
         <v>44591</v>
       </c>
-      <c r="H29" s="474">
+      <c r="H29" s="432">
         <v>19900</v>
       </c>
       <c r="I29" s="64">
@@ -4957,12 +4966,12 @@
         <f t="shared" si="1"/>
         <v>763700</v>
       </c>
-      <c r="O29" s="470"/>
-      <c r="P29" s="471"/>
-      <c r="Q29" s="472">
+      <c r="O29" s="428"/>
+      <c r="P29" s="429"/>
+      <c r="Q29" s="430">
         <v>25140</v>
       </c>
-      <c r="R29" s="473">
+      <c r="R29" s="431">
         <v>44596</v>
       </c>
       <c r="S29" s="91"/>
@@ -4994,7 +5003,7 @@
       <c r="G30" s="62">
         <v>44591</v>
       </c>
-      <c r="H30" s="474">
+      <c r="H30" s="432">
         <v>19900</v>
       </c>
       <c r="I30" s="64">
@@ -5013,12 +5022,12 @@
         <f t="shared" si="1"/>
         <v>190225</v>
       </c>
-      <c r="O30" s="470"/>
-      <c r="P30" s="471"/>
-      <c r="Q30" s="472">
-        <v>0</v>
-      </c>
-      <c r="R30" s="473">
+      <c r="O30" s="428"/>
+      <c r="P30" s="429"/>
+      <c r="Q30" s="430">
+        <v>0</v>
+      </c>
+      <c r="R30" s="431">
         <v>44596</v>
       </c>
       <c r="S30" s="91"/>
@@ -5890,13 +5899,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="463" t="s">
+      <c r="A56" s="433" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="465" t="s">
+      <c r="C56" s="435" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -5907,7 +5916,7 @@
       <c r="G56" s="152">
         <v>44571</v>
       </c>
-      <c r="H56" s="429">
+      <c r="H56" s="437">
         <v>782</v>
       </c>
       <c r="I56" s="151">
@@ -5936,11 +5945,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="464"/>
+      <c r="A57" s="434"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="466"/>
+      <c r="C57" s="436"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -5949,7 +5958,7 @@
       <c r="G57" s="152">
         <v>44571</v>
       </c>
-      <c r="H57" s="430"/>
+      <c r="H57" s="438"/>
       <c r="I57" s="151">
         <v>319</v>
       </c>
@@ -5976,13 +5985,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="451" t="s">
+      <c r="A58" s="464" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="453" t="s">
+      <c r="C58" s="462" t="s">
         <v>109</v>
       </c>
       <c r="D58" s="165"/>
@@ -5996,7 +6005,7 @@
       <c r="G58" s="152">
         <v>44585</v>
       </c>
-      <c r="H58" s="429">
+      <c r="H58" s="437">
         <v>800</v>
       </c>
       <c r="I58" s="151">
@@ -6015,10 +6024,10 @@
         <f t="shared" si="1"/>
         <v>151187.4</v>
       </c>
-      <c r="O58" s="459" t="s">
+      <c r="O58" s="465" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="460">
+      <c r="P58" s="467">
         <v>44594</v>
       </c>
       <c r="Q58" s="166"/>
@@ -6031,11 +6040,11 @@
       <c r="X58"/>
     </row>
     <row r="59" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="438"/>
+      <c r="A59" s="450"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="454"/>
+      <c r="C59" s="463"/>
       <c r="D59" s="167"/>
       <c r="E59" s="40">
         <f t="shared" si="2"/>
@@ -6047,7 +6056,7 @@
       <c r="G59" s="152">
         <v>44585</v>
       </c>
-      <c r="H59" s="430"/>
+      <c r="H59" s="438"/>
       <c r="I59" s="151">
         <v>231.6</v>
       </c>
@@ -6064,8 +6073,8 @@
         <f t="shared" si="1"/>
         <v>23623.200000000001</v>
       </c>
-      <c r="O59" s="461"/>
-      <c r="P59" s="462"/>
+      <c r="O59" s="466"/>
+      <c r="P59" s="468"/>
       <c r="Q59" s="166"/>
       <c r="R59" s="129"/>
       <c r="S59" s="92"/>
@@ -6074,11 +6083,11 @@
       <c r="V59" s="54"/>
     </row>
     <row r="60" spans="1:24" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="455"/>
+      <c r="A60" s="421"/>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="452"/>
+      <c r="C60" s="420"/>
       <c r="D60" s="167"/>
       <c r="E60" s="40">
         <f t="shared" si="2"/>
@@ -6086,7 +6095,7 @@
       </c>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="456"/>
+      <c r="H60" s="422"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -6099,8 +6108,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O60" s="457"/>
-      <c r="P60" s="458"/>
+      <c r="O60" s="423"/>
+      <c r="P60" s="424"/>
       <c r="Q60" s="166"/>
       <c r="R60" s="129"/>
       <c r="S60" s="92"/>
@@ -6109,11 +6118,11 @@
       <c r="V60" s="54"/>
     </row>
     <row r="61" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="437"/>
+      <c r="A61" s="449"/>
       <c r="B61" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="439"/>
+      <c r="C61" s="451"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -6121,7 +6130,7 @@
       </c>
       <c r="F61" s="151"/>
       <c r="G61" s="152"/>
-      <c r="H61" s="429"/>
+      <c r="H61" s="437"/>
       <c r="I61" s="151"/>
       <c r="J61" s="45">
         <f t="shared" si="0"/>
@@ -6146,11 +6155,11 @@
       <c r="X61"/>
     </row>
     <row r="62" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="438"/>
+      <c r="A62" s="450"/>
       <c r="B62" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="440"/>
+      <c r="C62" s="452"/>
       <c r="D62" s="170"/>
       <c r="E62" s="40">
         <f t="shared" si="2"/>
@@ -6158,7 +6167,7 @@
       </c>
       <c r="F62" s="151"/>
       <c r="G62" s="152"/>
-      <c r="H62" s="430"/>
+      <c r="H62" s="438"/>
       <c r="I62" s="151"/>
       <c r="J62" s="45">
         <f t="shared" si="0"/>
@@ -6336,8 +6345,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O66" s="431"/>
-      <c r="P66" s="433"/>
+      <c r="O66" s="441"/>
+      <c r="P66" s="453"/>
       <c r="Q66" s="166"/>
       <c r="R66" s="129"/>
       <c r="S66" s="182"/>
@@ -6371,8 +6380,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O67" s="441"/>
-      <c r="P67" s="442"/>
+      <c r="O67" s="442"/>
+      <c r="P67" s="454"/>
       <c r="Q67" s="166"/>
       <c r="R67" s="129"/>
       <c r="S67" s="182"/>
@@ -6561,10 +6570,10 @@
         <f t="shared" si="1"/>
         <v>13566</v>
       </c>
-      <c r="O71" s="467" t="s">
+      <c r="O71" s="425" t="s">
         <v>59</v>
       </c>
-      <c r="P71" s="468">
+      <c r="P71" s="426">
         <v>44595</v>
       </c>
       <c r="Q71" s="166"/>
@@ -6862,8 +6871,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="431"/>
-      <c r="P80" s="449"/>
+      <c r="O80" s="441"/>
+      <c r="P80" s="447"/>
       <c r="Q80" s="166"/>
       <c r="R80" s="129"/>
       <c r="S80" s="182"/>
@@ -6895,8 +6904,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="441"/>
-      <c r="P81" s="450"/>
+      <c r="O81" s="442"/>
+      <c r="P81" s="448"/>
       <c r="Q81" s="166"/>
       <c r="R81" s="129"/>
       <c r="S81" s="182"/>
@@ -6928,8 +6937,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="431"/>
-      <c r="P82" s="449"/>
+      <c r="O82" s="441"/>
+      <c r="P82" s="447"/>
       <c r="Q82" s="166"/>
       <c r="R82" s="158"/>
       <c r="S82" s="182"/>
@@ -6961,8 +6970,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="441"/>
-      <c r="P83" s="450"/>
+      <c r="O83" s="442"/>
+      <c r="P83" s="448"/>
       <c r="Q83" s="166"/>
       <c r="R83" s="158"/>
       <c r="S83" s="182"/>
@@ -7120,8 +7129,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="443"/>
-      <c r="M88" s="444"/>
+      <c r="L88" s="439"/>
+      <c r="M88" s="440"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7153,8 +7162,8 @@
         <v>0</v>
       </c>
       <c r="K89" s="100"/>
-      <c r="L89" s="443"/>
-      <c r="M89" s="444"/>
+      <c r="L89" s="439"/>
+      <c r="M89" s="440"/>
       <c r="N89" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7357,8 +7366,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="431"/>
-      <c r="P95" s="445"/>
+      <c r="O95" s="441"/>
+      <c r="P95" s="443"/>
       <c r="Q95" s="166"/>
       <c r="R95" s="129"/>
       <c r="S95" s="182"/>
@@ -7390,8 +7399,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O96" s="441"/>
-      <c r="P96" s="446"/>
+      <c r="O96" s="442"/>
+      <c r="P96" s="444"/>
       <c r="Q96" s="166"/>
       <c r="R96" s="129"/>
       <c r="S96" s="182"/>
@@ -12783,11 +12792,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F260" s="447" t="s">
+      <c r="F260" s="445" t="s">
         <v>26</v>
       </c>
-      <c r="G260" s="447"/>
-      <c r="H260" s="448"/>
+      <c r="G260" s="445"/>
+      <c r="H260" s="446"/>
       <c r="I260" s="319">
         <f>SUM(I4:I259)</f>
         <v>423660.27</v>
@@ -13361,21 +13370,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="L88:M89"/>
-    <mergeCell ref="O95:O96"/>
-    <mergeCell ref="P95:P96"/>
-    <mergeCell ref="F260:H260"/>
-    <mergeCell ref="O80:O81"/>
-    <mergeCell ref="P80:P81"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="O66:O67"/>
     <mergeCell ref="P66:P67"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
@@ -13386,6 +13380,21 @@
     <mergeCell ref="H58:H59"/>
     <mergeCell ref="O58:O59"/>
     <mergeCell ref="P58:P59"/>
+    <mergeCell ref="P95:P96"/>
+    <mergeCell ref="F260:H260"/>
+    <mergeCell ref="O80:O81"/>
+    <mergeCell ref="P80:P81"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="L88:M89"/>
+    <mergeCell ref="O95:O96"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="O66:O67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13400,10 +13409,10 @@
   <dimension ref="A1:X291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13432,18 +13441,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="420" t="s">
+      <c r="A1" s="455" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="420"/>
-      <c r="C1" s="420"/>
-      <c r="D1" s="420"/>
-      <c r="E1" s="420"/>
-      <c r="F1" s="420"/>
-      <c r="G1" s="420"/>
-      <c r="H1" s="420"/>
-      <c r="I1" s="420"/>
-      <c r="J1" s="420"/>
+      <c r="B1" s="455"/>
+      <c r="C1" s="455"/>
+      <c r="D1" s="455"/>
+      <c r="E1" s="455"/>
+      <c r="F1" s="455"/>
+      <c r="G1" s="455"/>
+      <c r="H1" s="455"/>
+      <c r="I1" s="455"/>
+      <c r="J1" s="455"/>
       <c r="K1" s="377"/>
       <c r="L1" s="377"/>
       <c r="M1" s="377"/>
@@ -13457,22 +13466,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="421" t="s">
+      <c r="W1" s="456" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="422"/>
+      <c r="X1" s="457"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="420"/>
-      <c r="B2" s="420"/>
-      <c r="C2" s="420"/>
-      <c r="D2" s="420"/>
-      <c r="E2" s="420"/>
-      <c r="F2" s="420"/>
-      <c r="G2" s="420"/>
-      <c r="H2" s="420"/>
-      <c r="I2" s="420"/>
-      <c r="J2" s="420"/>
+      <c r="A2" s="455"/>
+      <c r="B2" s="455"/>
+      <c r="C2" s="455"/>
+      <c r="D2" s="455"/>
+      <c r="E2" s="455"/>
+      <c r="F2" s="455"/>
+      <c r="G2" s="455"/>
+      <c r="H2" s="455"/>
+      <c r="I2" s="455"/>
+      <c r="J2" s="455"/>
       <c r="K2" s="379"/>
       <c r="L2" s="379"/>
       <c r="M2" s="379"/>
@@ -13526,10 +13535,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="423" t="s">
+      <c r="O3" s="458" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="424"/>
+      <c r="P3" s="459"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -14184,25 +14193,37 @@
       <c r="X16" s="70"/>
     </row>
     <row r="17" spans="1:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="75"/>
-      <c r="B17" s="58"/>
+      <c r="A17" s="75" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>31</v>
+      </c>
       <c r="C17" s="59"/>
       <c r="D17" s="60"/>
       <c r="E17" s="40"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="62"/>
+      <c r="F17" s="61">
+        <v>17220</v>
+      </c>
+      <c r="G17" s="62">
+        <v>44605</v>
+      </c>
       <c r="H17" s="413"/>
-      <c r="I17" s="414"/>
+      <c r="I17" s="414">
+        <v>21340</v>
+      </c>
       <c r="J17" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="76"/>
+        <v>4120</v>
+      </c>
+      <c r="K17" s="76">
+        <v>33.5</v>
+      </c>
       <c r="L17" s="65"/>
       <c r="M17" s="65"/>
       <c r="N17" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>714890</v>
       </c>
       <c r="O17" s="399"/>
       <c r="P17" s="400"/>
@@ -14218,25 +14239,37 @@
       <c r="X17" s="70"/>
     </row>
     <row r="18" spans="1:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="78"/>
-      <c r="B18" s="58"/>
+      <c r="A18" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>72</v>
+      </c>
       <c r="C18" s="59"/>
       <c r="D18" s="60"/>
       <c r="E18" s="40"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="62"/>
+      <c r="F18" s="61">
+        <v>20360</v>
+      </c>
+      <c r="G18" s="62">
+        <v>44607</v>
+      </c>
       <c r="H18" s="413"/>
-      <c r="I18" s="414"/>
+      <c r="I18" s="414">
+        <v>20110</v>
+      </c>
       <c r="J18" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="76"/>
+        <v>-250</v>
+      </c>
+      <c r="K18" s="76">
+        <v>32.75</v>
+      </c>
       <c r="L18" s="65"/>
       <c r="M18" s="65"/>
       <c r="N18" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>658602.5</v>
       </c>
       <c r="O18" s="399"/>
       <c r="P18" s="400"/>
@@ -14250,25 +14283,37 @@
       <c r="X18" s="70"/>
     </row>
     <row r="19" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="78"/>
-      <c r="B19" s="58"/>
+      <c r="A19" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>32</v>
+      </c>
       <c r="C19" s="59"/>
       <c r="D19" s="60"/>
       <c r="E19" s="40"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="62"/>
+      <c r="F19" s="61">
+        <v>0</v>
+      </c>
+      <c r="G19" s="62">
+        <v>44607</v>
+      </c>
       <c r="H19" s="413"/>
-      <c r="I19" s="414"/>
+      <c r="I19" s="414">
+        <v>5175</v>
+      </c>
       <c r="J19" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="76"/>
+        <v>5175</v>
+      </c>
+      <c r="K19" s="76">
+        <v>32.75</v>
+      </c>
       <c r="L19" s="65"/>
       <c r="M19" s="65"/>
       <c r="N19" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>169481.25</v>
       </c>
       <c r="O19" s="399"/>
       <c r="P19" s="400"/>
@@ -14282,25 +14327,37 @@
       <c r="X19" s="70"/>
     </row>
     <row r="20" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="80"/>
-      <c r="B20" s="58"/>
+      <c r="A20" s="80" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="58" t="s">
+        <v>129</v>
+      </c>
       <c r="C20" s="59"/>
       <c r="D20" s="60"/>
       <c r="E20" s="40"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="62"/>
+      <c r="F20" s="61">
+        <v>21610</v>
+      </c>
+      <c r="G20" s="62">
+        <v>44609</v>
+      </c>
       <c r="H20" s="413"/>
-      <c r="I20" s="414"/>
+      <c r="I20" s="414">
+        <v>21115</v>
+      </c>
       <c r="J20" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="76"/>
+        <v>-495</v>
+      </c>
+      <c r="K20" s="76">
+        <v>32.75</v>
+      </c>
       <c r="L20" s="65"/>
       <c r="M20" s="65"/>
       <c r="N20" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>691516.25</v>
       </c>
       <c r="O20" s="89"/>
       <c r="P20" s="90"/>
@@ -14314,25 +14371,37 @@
       <c r="X20" s="70"/>
     </row>
     <row r="21" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="78"/>
-      <c r="B21" s="58"/>
+      <c r="A21" s="78" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="58" t="s">
+        <v>32</v>
+      </c>
       <c r="C21" s="59"/>
       <c r="D21" s="60"/>
       <c r="E21" s="40"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="62"/>
+      <c r="F21" s="61">
+        <v>0</v>
+      </c>
+      <c r="G21" s="62">
+        <v>44609</v>
+      </c>
       <c r="H21" s="413"/>
-      <c r="I21" s="414"/>
+      <c r="I21" s="414">
+        <v>5780</v>
+      </c>
       <c r="J21" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="76"/>
+        <v>5780</v>
+      </c>
+      <c r="K21" s="76">
+        <v>32.75</v>
+      </c>
       <c r="L21" s="65"/>
       <c r="M21" s="65"/>
       <c r="N21" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>189295</v>
       </c>
       <c r="O21" s="89"/>
       <c r="P21" s="90"/>
@@ -14346,25 +14415,37 @@
       <c r="X21" s="70"/>
     </row>
     <row r="22" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="81"/>
-      <c r="B22" s="58"/>
+      <c r="A22" s="81" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>72</v>
+      </c>
       <c r="C22" s="59"/>
       <c r="D22" s="60"/>
       <c r="E22" s="40"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="62"/>
+      <c r="F22" s="61">
+        <v>21980</v>
+      </c>
+      <c r="G22" s="62">
+        <v>44610</v>
+      </c>
       <c r="H22" s="413"/>
-      <c r="I22" s="414"/>
+      <c r="I22" s="414">
+        <v>22560</v>
+      </c>
       <c r="J22" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="76"/>
+        <v>580</v>
+      </c>
+      <c r="K22" s="76">
+        <v>32.75</v>
+      </c>
       <c r="L22" s="65"/>
       <c r="M22" s="65"/>
       <c r="N22" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>738840</v>
       </c>
       <c r="O22" s="89"/>
       <c r="P22" s="90"/>
@@ -14378,25 +14459,37 @@
       <c r="X22" s="70"/>
     </row>
     <row r="23" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="82"/>
-      <c r="B23" s="58"/>
+      <c r="A23" s="82" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="58" t="s">
+        <v>32</v>
+      </c>
       <c r="C23" s="59"/>
       <c r="D23" s="60"/>
       <c r="E23" s="40"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="62"/>
+      <c r="F23" s="61">
+        <v>0</v>
+      </c>
+      <c r="G23" s="62">
+        <v>44610</v>
+      </c>
       <c r="H23" s="413"/>
-      <c r="I23" s="414"/>
+      <c r="I23" s="414">
+        <v>5550</v>
+      </c>
       <c r="J23" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="76"/>
+        <v>5550</v>
+      </c>
+      <c r="K23" s="76">
+        <v>32.75</v>
+      </c>
       <c r="L23" s="65"/>
       <c r="M23" s="65"/>
       <c r="N23" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>181762.5</v>
       </c>
       <c r="O23" s="89"/>
       <c r="P23" s="90"/>
@@ -15501,16 +15594,16 @@
       <c r="X56"/>
     </row>
     <row r="57" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="425"/>
+      <c r="A57" s="469"/>
       <c r="B57" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="427"/>
+      <c r="C57" s="471"/>
       <c r="D57" s="167"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151"/>
       <c r="G57" s="152"/>
-      <c r="H57" s="429"/>
+      <c r="H57" s="437"/>
       <c r="I57" s="151"/>
       <c r="J57" s="45">
         <f t="shared" si="0"/>
@@ -15523,8 +15616,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O57" s="431"/>
-      <c r="P57" s="433"/>
+      <c r="O57" s="441"/>
+      <c r="P57" s="453"/>
       <c r="Q57" s="166"/>
       <c r="R57" s="129"/>
       <c r="S57" s="92"/>
@@ -15533,16 +15626,16 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="426"/>
+      <c r="A58" s="470"/>
       <c r="B58" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="428"/>
+      <c r="C58" s="472"/>
       <c r="D58" s="167"/>
       <c r="E58" s="40"/>
       <c r="F58" s="151"/>
       <c r="G58" s="152"/>
-      <c r="H58" s="430"/>
+      <c r="H58" s="438"/>
       <c r="I58" s="151"/>
       <c r="J58" s="45">
         <f t="shared" si="0"/>
@@ -15555,8 +15648,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O58" s="432"/>
-      <c r="P58" s="434"/>
+      <c r="O58" s="473"/>
+      <c r="P58" s="474"/>
       <c r="Q58" s="166"/>
       <c r="R58" s="129"/>
       <c r="S58" s="92"/>
@@ -15565,16 +15658,16 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="437"/>
+      <c r="A59" s="449"/>
       <c r="B59" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="439"/>
+      <c r="C59" s="451"/>
       <c r="D59" s="165"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151"/>
       <c r="G59" s="152"/>
-      <c r="H59" s="429"/>
+      <c r="H59" s="437"/>
       <c r="I59" s="151"/>
       <c r="J59" s="45">
         <f t="shared" si="0"/>
@@ -15599,16 +15692,16 @@
       <c r="X59"/>
     </row>
     <row r="60" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="438"/>
+      <c r="A60" s="450"/>
       <c r="B60" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="440"/>
+      <c r="C60" s="452"/>
       <c r="D60" s="170"/>
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="430"/>
+      <c r="H60" s="438"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -15745,8 +15838,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O64" s="431"/>
-      <c r="P64" s="433"/>
+      <c r="O64" s="441"/>
+      <c r="P64" s="453"/>
       <c r="Q64" s="166"/>
       <c r="R64" s="129"/>
       <c r="S64" s="182"/>
@@ -15775,8 +15868,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O65" s="441"/>
-      <c r="P65" s="442"/>
+      <c r="O65" s="442"/>
+      <c r="P65" s="454"/>
       <c r="Q65" s="166"/>
       <c r="R65" s="129"/>
       <c r="S65" s="182"/>
@@ -16173,8 +16266,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O78" s="431"/>
-      <c r="P78" s="449"/>
+      <c r="O78" s="441"/>
+      <c r="P78" s="447"/>
       <c r="Q78" s="166"/>
       <c r="R78" s="129"/>
       <c r="S78" s="182"/>
@@ -16203,8 +16296,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="441"/>
-      <c r="P79" s="450"/>
+      <c r="O79" s="442"/>
+      <c r="P79" s="448"/>
       <c r="Q79" s="166"/>
       <c r="R79" s="129"/>
       <c r="S79" s="182"/>
@@ -16233,8 +16326,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="431"/>
-      <c r="P80" s="449"/>
+      <c r="O80" s="441"/>
+      <c r="P80" s="447"/>
       <c r="Q80" s="166"/>
       <c r="R80" s="158"/>
       <c r="S80" s="182"/>
@@ -16266,8 +16359,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="441"/>
-      <c r="P81" s="450"/>
+      <c r="O81" s="442"/>
+      <c r="P81" s="448"/>
       <c r="Q81" s="166"/>
       <c r="R81" s="158"/>
       <c r="S81" s="182"/>
@@ -16425,8 +16518,8 @@
         <v>0</v>
       </c>
       <c r="K86" s="100"/>
-      <c r="L86" s="443"/>
-      <c r="M86" s="444"/>
+      <c r="L86" s="439"/>
+      <c r="M86" s="440"/>
       <c r="N86" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -16458,8 +16551,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="443"/>
-      <c r="M87" s="444"/>
+      <c r="L87" s="439"/>
+      <c r="M87" s="440"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -16662,8 +16755,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O93" s="431"/>
-      <c r="P93" s="445"/>
+      <c r="O93" s="441"/>
+      <c r="P93" s="443"/>
       <c r="Q93" s="166"/>
       <c r="R93" s="129"/>
       <c r="S93" s="182"/>
@@ -16695,8 +16788,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="441"/>
-      <c r="P94" s="446"/>
+      <c r="O94" s="442"/>
+      <c r="P94" s="444"/>
       <c r="Q94" s="166"/>
       <c r="R94" s="129"/>
       <c r="S94" s="182"/>
@@ -22088,14 +22181,14 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F258" s="447" t="s">
+      <c r="F258" s="445" t="s">
         <v>26</v>
       </c>
-      <c r="G258" s="447"/>
-      <c r="H258" s="448"/>
+      <c r="G258" s="445"/>
+      <c r="H258" s="446"/>
       <c r="I258" s="319">
         <f>SUM(I4:I257)</f>
-        <v>172025</v>
+        <v>273655</v>
       </c>
       <c r="J258" s="320"/>
       <c r="K258" s="316"/>
@@ -22194,7 +22287,7 @@
       <c r="M262" s="338"/>
       <c r="N262" s="339">
         <f>SUM(N4:N261)</f>
-        <v>5951597.5</v>
+        <v>9295985</v>
       </c>
       <c r="O262" s="340"/>
       <c r="Q262" s="341">
@@ -22254,7 +22347,7 @@
       <c r="M265" s="354"/>
       <c r="N265" s="355">
         <f>V262+S262+Q262+N262+L262</f>
-        <v>6102537.5</v>
+        <v>9446925</v>
       </c>
       <c r="O265" s="356"/>
       <c r="R265" s="326"/>
@@ -22666,6 +22759,16 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="P80:P81"/>
+    <mergeCell ref="L86:M87"/>
+    <mergeCell ref="O93:O94"/>
+    <mergeCell ref="P93:P94"/>
+    <mergeCell ref="F258:H258"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="O64:O65"/>
+    <mergeCell ref="O80:O81"/>
     <mergeCell ref="P64:P65"/>
     <mergeCell ref="O78:O79"/>
     <mergeCell ref="P78:P79"/>
@@ -22677,16 +22780,6 @@
     <mergeCell ref="H57:H58"/>
     <mergeCell ref="O57:O58"/>
     <mergeCell ref="P57:P58"/>
-    <mergeCell ref="F258:H258"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="O64:O65"/>
-    <mergeCell ref="O80:O81"/>
-    <mergeCell ref="P80:P81"/>
-    <mergeCell ref="L86:M87"/>
-    <mergeCell ref="O93:O94"/>
-    <mergeCell ref="P93:P94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 8 DE MAR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/ENTRADAS OBRADOR FEBRERO  2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/ENTRADAS OBRADOR FEBRERO  2022.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="188">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -581,6 +581,15 @@
   </si>
   <si>
     <t>0164 Z</t>
+  </si>
+  <si>
+    <t>0174 Z</t>
+  </si>
+  <si>
+    <t>0190 Z</t>
+  </si>
+  <si>
+    <t>0208 Z</t>
   </si>
 </sst>
 </file>
@@ -3058,6 +3067,81 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3091,83 +3175,14 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3197,12 +3212,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3533,18 +3542,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="433" t="s">
+      <c r="A1" s="458" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="433"/>
-      <c r="C1" s="433"/>
-      <c r="D1" s="433"/>
-      <c r="E1" s="433"/>
-      <c r="F1" s="433"/>
-      <c r="G1" s="433"/>
-      <c r="H1" s="433"/>
-      <c r="I1" s="433"/>
-      <c r="J1" s="433"/>
+      <c r="B1" s="458"/>
+      <c r="C1" s="458"/>
+      <c r="D1" s="458"/>
+      <c r="E1" s="458"/>
+      <c r="F1" s="458"/>
+      <c r="G1" s="458"/>
+      <c r="H1" s="458"/>
+      <c r="I1" s="458"/>
+      <c r="J1" s="458"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -3558,22 +3567,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="434" t="s">
+      <c r="W1" s="459" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="435"/>
+      <c r="X1" s="460"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="433"/>
-      <c r="B2" s="433"/>
-      <c r="C2" s="433"/>
-      <c r="D2" s="433"/>
-      <c r="E2" s="433"/>
-      <c r="F2" s="433"/>
-      <c r="G2" s="433"/>
-      <c r="H2" s="433"/>
-      <c r="I2" s="433"/>
-      <c r="J2" s="433"/>
+      <c r="A2" s="458"/>
+      <c r="B2" s="458"/>
+      <c r="C2" s="458"/>
+      <c r="D2" s="458"/>
+      <c r="E2" s="458"/>
+      <c r="F2" s="458"/>
+      <c r="G2" s="458"/>
+      <c r="H2" s="458"/>
+      <c r="I2" s="458"/>
+      <c r="J2" s="458"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -3627,10 +3636,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="436" t="s">
+      <c r="O3" s="461" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="437"/>
+      <c r="P3" s="462"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -4174,7 +4183,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="438" t="s">
+      <c r="C12" s="463" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -4238,7 +4247,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="439"/>
+      <c r="C13" s="464"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -6240,13 +6249,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="450" t="s">
+      <c r="A56" s="442" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="452" t="s">
+      <c r="C56" s="444" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -6257,7 +6266,7 @@
       <c r="G56" s="152">
         <v>44571</v>
       </c>
-      <c r="H56" s="444">
+      <c r="H56" s="446">
         <v>782</v>
       </c>
       <c r="I56" s="151">
@@ -6286,11 +6295,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="451"/>
+      <c r="A57" s="443"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="453"/>
+      <c r="C57" s="445"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -6299,7 +6308,7 @@
       <c r="G57" s="152">
         <v>44571</v>
       </c>
-      <c r="H57" s="445"/>
+      <c r="H57" s="447"/>
       <c r="I57" s="151">
         <v>319</v>
       </c>
@@ -6326,13 +6335,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="450" t="s">
+      <c r="A58" s="442" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="452" t="s">
+      <c r="C58" s="444" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -6343,7 +6352,7 @@
       <c r="G58" s="152">
         <v>44578</v>
       </c>
-      <c r="H58" s="444">
+      <c r="H58" s="446">
         <v>810</v>
       </c>
       <c r="I58" s="151">
@@ -6362,10 +6371,10 @@
         <f t="shared" si="1"/>
         <v>75875.8</v>
       </c>
-      <c r="O58" s="446" t="s">
+      <c r="O58" s="448" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="448">
+      <c r="P58" s="469">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -6376,11 +6385,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="451"/>
+      <c r="A59" s="443"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="453"/>
+      <c r="C59" s="445"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -6389,7 +6398,7 @@
       <c r="G59" s="152">
         <v>44578</v>
       </c>
-      <c r="H59" s="445"/>
+      <c r="H59" s="447"/>
       <c r="I59" s="151">
         <v>220</v>
       </c>
@@ -6406,8 +6415,8 @@
         <f t="shared" si="1"/>
         <v>22440</v>
       </c>
-      <c r="O59" s="447"/>
-      <c r="P59" s="449"/>
+      <c r="O59" s="449"/>
+      <c r="P59" s="470"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -6416,13 +6425,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="442" t="s">
+      <c r="A60" s="467" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="440" t="s">
+      <c r="C60" s="465" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -6436,7 +6445,7 @@
       <c r="G60" s="152">
         <v>44585</v>
       </c>
-      <c r="H60" s="444">
+      <c r="H60" s="446">
         <v>800</v>
       </c>
       <c r="I60" s="151">
@@ -6455,10 +6464,10 @@
         <f t="shared" si="1"/>
         <v>151187.4</v>
       </c>
-      <c r="O60" s="446" t="s">
+      <c r="O60" s="448" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="448">
+      <c r="P60" s="469">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -6471,11 +6480,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="443"/>
+      <c r="A61" s="468"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="441"/>
+      <c r="C61" s="466"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -6487,7 +6496,7 @@
       <c r="G61" s="152">
         <v>44585</v>
       </c>
-      <c r="H61" s="445"/>
+      <c r="H61" s="447"/>
       <c r="I61" s="151">
         <v>231.6</v>
       </c>
@@ -6504,8 +6513,8 @@
         <f t="shared" si="1"/>
         <v>23623.200000000001</v>
       </c>
-      <c r="O61" s="447"/>
-      <c r="P61" s="449"/>
+      <c r="O61" s="449"/>
+      <c r="P61" s="470"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -6571,7 +6580,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="466"/>
+      <c r="C63" s="436"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -6579,7 +6588,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="468"/>
+      <c r="H63" s="438"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -6608,7 +6617,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="467"/>
+      <c r="C64" s="437"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -6616,7 +6625,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="469"/>
+      <c r="H64" s="439"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -6794,8 +6803,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="458"/>
-      <c r="P68" s="464"/>
+      <c r="O68" s="440"/>
+      <c r="P68" s="434"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -6829,8 +6838,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="459"/>
-      <c r="P69" s="465"/>
+      <c r="O69" s="441"/>
+      <c r="P69" s="435"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -7320,8 +7329,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="458"/>
-      <c r="P82" s="460"/>
+      <c r="O82" s="440"/>
+      <c r="P82" s="454"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -7353,8 +7362,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="459"/>
-      <c r="P83" s="461"/>
+      <c r="O83" s="441"/>
+      <c r="P83" s="455"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -7386,8 +7395,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="458"/>
-      <c r="P84" s="460"/>
+      <c r="O84" s="440"/>
+      <c r="P84" s="454"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -7419,8 +7428,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="459"/>
-      <c r="P85" s="461"/>
+      <c r="O85" s="441"/>
+      <c r="P85" s="455"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -7578,8 +7587,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="462"/>
-      <c r="M90" s="463"/>
+      <c r="L90" s="456"/>
+      <c r="M90" s="457"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7611,8 +7620,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="462"/>
-      <c r="M91" s="463"/>
+      <c r="L91" s="456"/>
+      <c r="M91" s="457"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7815,8 +7824,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="458"/>
-      <c r="P97" s="454"/>
+      <c r="O97" s="440"/>
+      <c r="P97" s="450"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -7848,8 +7857,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="459"/>
-      <c r="P98" s="455"/>
+      <c r="O98" s="441"/>
+      <c r="P98" s="451"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -13241,11 +13250,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="456" t="s">
+      <c r="F262" s="452" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="456"/>
-      <c r="H262" s="457"/>
+      <c r="G262" s="452"/>
+      <c r="H262" s="453"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -13819,22 +13828,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -13848,6 +13841,22 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13862,10 +13871,10 @@
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="V8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="V11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13894,49 +13903,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="433" t="s">
+      <c r="A1" s="458" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="433"/>
-      <c r="C1" s="433"/>
-      <c r="D1" s="433"/>
-      <c r="E1" s="433"/>
-      <c r="F1" s="433"/>
-      <c r="G1" s="433"/>
-      <c r="H1" s="433"/>
-      <c r="I1" s="433"/>
-      <c r="J1" s="433"/>
+      <c r="B1" s="458"/>
+      <c r="C1" s="458"/>
+      <c r="D1" s="458"/>
+      <c r="E1" s="458"/>
+      <c r="F1" s="458"/>
+      <c r="G1" s="458"/>
+      <c r="H1" s="458"/>
+      <c r="I1" s="458"/>
+      <c r="J1" s="458"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="476" t="s">
+      <c r="S1" s="478" t="s">
         <v>143</v>
       </c>
-      <c r="T1" s="476"/>
+      <c r="T1" s="478"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="434" t="s">
+      <c r="W1" s="459" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="435"/>
+      <c r="X1" s="460"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="433"/>
-      <c r="B2" s="433"/>
-      <c r="C2" s="433"/>
-      <c r="D2" s="433"/>
-      <c r="E2" s="433"/>
-      <c r="F2" s="433"/>
-      <c r="G2" s="433"/>
-      <c r="H2" s="433"/>
-      <c r="I2" s="433"/>
-      <c r="J2" s="433"/>
+      <c r="A2" s="458"/>
+      <c r="B2" s="458"/>
+      <c r="C2" s="458"/>
+      <c r="D2" s="458"/>
+      <c r="E2" s="458"/>
+      <c r="F2" s="458"/>
+      <c r="G2" s="458"/>
+      <c r="H2" s="458"/>
+      <c r="I2" s="458"/>
+      <c r="J2" s="458"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -13944,8 +13953,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="477"/>
-      <c r="T2" s="477"/>
+      <c r="S2" s="479"/>
+      <c r="T2" s="479"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -13990,10 +13999,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="436" t="s">
+      <c r="O3" s="461" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="437"/>
+      <c r="P3" s="462"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -14562,7 +14571,7 @@
       <c r="B13" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="481" t="s">
+      <c r="C13" s="433" t="s">
         <v>184</v>
       </c>
       <c r="D13" s="60"/>
@@ -14682,7 +14691,9 @@
       <c r="B15" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="59"/>
+      <c r="C15" s="59" t="s">
+        <v>185</v>
+      </c>
       <c r="D15" s="60"/>
       <c r="E15" s="40"/>
       <c r="F15" s="61">
@@ -14740,7 +14751,9 @@
       <c r="B16" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="74" t="s">
+        <v>185</v>
+      </c>
       <c r="D16" s="60"/>
       <c r="E16" s="40"/>
       <c r="F16" s="61">
@@ -14798,7 +14811,9 @@
       <c r="B17" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="59"/>
+      <c r="C17" s="59" t="s">
+        <v>186</v>
+      </c>
       <c r="D17" s="60"/>
       <c r="E17" s="40"/>
       <c r="F17" s="61">
@@ -14860,7 +14875,9 @@
       <c r="B18" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="59"/>
+      <c r="C18" s="59" t="s">
+        <v>187</v>
+      </c>
       <c r="D18" s="60"/>
       <c r="E18" s="40"/>
       <c r="F18" s="61">
@@ -14922,7 +14939,9 @@
       <c r="B19" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="59"/>
+      <c r="C19" s="59" t="s">
+        <v>187</v>
+      </c>
       <c r="D19" s="60"/>
       <c r="E19" s="40"/>
       <c r="F19" s="61">
@@ -16419,13 +16438,13 @@
       <c r="V54" s="160"/>
     </row>
     <row r="55" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="478" t="s">
+      <c r="A55" s="480" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="452" t="s">
+      <c r="C55" s="444" t="s">
         <v>161</v>
       </c>
       <c r="D55" s="150"/>
@@ -16436,7 +16455,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="468" t="s">
+      <c r="H55" s="438" t="s">
         <v>162</v>
       </c>
       <c r="I55" s="151">
@@ -16465,11 +16484,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="479"/>
+      <c r="A56" s="481"/>
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="453"/>
+      <c r="C56" s="445"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -16478,7 +16497,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="469"/>
+      <c r="H56" s="439"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -16507,13 +16526,13 @@
       <c r="X56"/>
     </row>
     <row r="57" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="470" t="s">
+      <c r="A57" s="472" t="s">
         <v>41</v>
       </c>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="472" t="s">
+      <c r="C57" s="474" t="s">
         <v>163</v>
       </c>
       <c r="D57" s="165"/>
@@ -16524,7 +16543,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="468" t="s">
+      <c r="H57" s="438" t="s">
         <v>164</v>
       </c>
       <c r="I57" s="151">
@@ -16543,10 +16562,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="458" t="s">
+      <c r="O57" s="440" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="464">
+      <c r="P57" s="434">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -16557,11 +16576,11 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="471"/>
+      <c r="A58" s="473"/>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="473"/>
+      <c r="C58" s="475"/>
       <c r="D58" s="165"/>
       <c r="E58" s="40"/>
       <c r="F58" s="151">
@@ -16570,7 +16589,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="469"/>
+      <c r="H58" s="439"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -16587,8 +16606,8 @@
         <f t="shared" si="1"/>
         <v>58366.995299999995</v>
       </c>
-      <c r="O58" s="474"/>
-      <c r="P58" s="475"/>
+      <c r="O58" s="476"/>
+      <c r="P58" s="477"/>
       <c r="Q58" s="164"/>
       <c r="R58" s="129"/>
       <c r="S58" s="92"/>
@@ -16597,16 +16616,16 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="480"/>
+      <c r="A59" s="471"/>
       <c r="B59" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="466"/>
+      <c r="C59" s="436"/>
       <c r="D59" s="163"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151"/>
       <c r="G59" s="152"/>
-      <c r="H59" s="468"/>
+      <c r="H59" s="438"/>
       <c r="I59" s="151"/>
       <c r="J59" s="45">
         <f t="shared" si="0"/>
@@ -16631,16 +16650,16 @@
       <c r="X59"/>
     </row>
     <row r="60" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="443"/>
+      <c r="A60" s="468"/>
       <c r="B60" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="467"/>
+      <c r="C60" s="437"/>
       <c r="D60" s="168"/>
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="469"/>
+      <c r="H60" s="439"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -16863,8 +16882,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O65" s="458"/>
-      <c r="P65" s="464"/>
+      <c r="O65" s="440"/>
+      <c r="P65" s="434"/>
       <c r="Q65" s="164"/>
       <c r="R65" s="129"/>
       <c r="S65" s="180"/>
@@ -16893,8 +16912,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O66" s="459"/>
-      <c r="P66" s="465"/>
+      <c r="O66" s="441"/>
+      <c r="P66" s="435"/>
       <c r="Q66" s="164"/>
       <c r="R66" s="129"/>
       <c r="S66" s="180"/>
@@ -17283,8 +17302,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="458"/>
-      <c r="P79" s="460"/>
+      <c r="O79" s="440"/>
+      <c r="P79" s="454"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -17313,8 +17332,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="459"/>
-      <c r="P80" s="461"/>
+      <c r="O80" s="441"/>
+      <c r="P80" s="455"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -17343,8 +17362,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="458"/>
-      <c r="P81" s="460"/>
+      <c r="O81" s="440"/>
+      <c r="P81" s="454"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -17376,8 +17395,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="459"/>
-      <c r="P82" s="461"/>
+      <c r="O82" s="441"/>
+      <c r="P82" s="455"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -17535,8 +17554,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="462"/>
-      <c r="M87" s="463"/>
+      <c r="L87" s="456"/>
+      <c r="M87" s="457"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -17568,8 +17587,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="462"/>
-      <c r="M88" s="463"/>
+      <c r="L88" s="456"/>
+      <c r="M88" s="457"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -17772,8 +17791,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="458"/>
-      <c r="P94" s="454"/>
+      <c r="O94" s="440"/>
+      <c r="P94" s="450"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -17805,8 +17824,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="459"/>
-      <c r="P95" s="455"/>
+      <c r="O95" s="441"/>
+      <c r="P95" s="451"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -23198,11 +23217,11 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="456" t="s">
+      <c r="F259" s="452" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="456"/>
-      <c r="H259" s="457"/>
+      <c r="G259" s="452"/>
+      <c r="H259" s="453"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>385569.10210000002</v>
@@ -23776,14 +23795,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="P65:P66"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="O65:O66"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="A57:A58"/>
@@ -23795,12 +23812,14 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
+    <mergeCell ref="P65:P66"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="O65:O66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>